<commit_message>
tweaked the model and collected time-domain results
changed a bit on the parameters of speed governor
</commit_message>
<xml_diff>
--- a/system_cases/IMR_case/IEEE68_bad.xlsx
+++ b/system_cases/IMR_case/IEEE68_bad.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitRep\Simplus-Grid-Tool\system_cases\IMR_case\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Simplus-Grid-Tool\system_cases\IMR_case\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F88E33B-8979-4DC9-8039-07164523335C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01ACB3E9-FE8E-43AE-B2BE-85CD9868B861}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -125,7 +125,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{5C619B6F-3B70-437D-80F8-7830CA671B59}">
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{D4E2DABB-2EBB-4914-B2B9-C70CEF73F27E}">
       <text>
         <r>
           <rPr>
@@ -1159,8 +1159,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L70"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F61" sqref="F61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2522,7 +2522,7 @@
         <v>2</v>
       </c>
       <c r="F37" s="24">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="G37" s="7">
         <v>0</v>
@@ -2674,7 +2674,7 @@
         <v>5</v>
       </c>
       <c r="F41" s="24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G41" s="7">
         <v>2.67</v>
@@ -2826,7 +2826,7 @@
         <v>5</v>
       </c>
       <c r="F45" s="24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G45" s="7">
         <v>0</v>
@@ -2864,7 +2864,7 @@
         <v>5</v>
       </c>
       <c r="F46" s="24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G46" s="7">
         <v>2.6755</v>
@@ -2902,7 +2902,7 @@
         <v>3</v>
       </c>
       <c r="F47" s="14">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="G47" s="7">
         <v>2.08</v>
@@ -3092,7 +3092,7 @@
         <v>4</v>
       </c>
       <c r="F52" s="24">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="G52" s="7">
         <v>1</v>
@@ -3130,7 +3130,7 @@
         <v>4</v>
       </c>
       <c r="F53" s="24">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="G53" s="7">
         <v>3.37</v>
@@ -3396,7 +3396,7 @@
         <v>1</v>
       </c>
       <c r="F60">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="G60">
         <v>0</v>
@@ -3434,7 +3434,7 @@
         <v>1</v>
       </c>
       <c r="F61">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="G61">
         <v>2.34</v>
@@ -3809,8 +3809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34645F5B-1D7A-4323-9AD6-5FF81941CA24}">
   <dimension ref="A1:AQ73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I48" sqref="I48:I50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4094,7 +4094,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="49">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C6" s="44">
         <v>2.0500000000000002E-3</v>
@@ -4144,7 +4144,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="43">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C7" s="16">
         <v>3.5000000000000003E-2</v>
@@ -4275,7 +4275,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="43">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C8" s="16">
         <v>3.04E-2</v>
@@ -4406,7 +4406,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="43">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C9" s="16">
         <v>2.9499999999999998E-2</v>
@@ -4537,7 +4537,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="43">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C10" s="16">
         <v>2.7E-2</v>
@@ -4668,7 +4668,7 @@
         <v>6</v>
       </c>
       <c r="B11" s="43">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C11" s="16">
         <v>2.24E-2</v>
@@ -4799,7 +4799,7 @@
         <v>7</v>
       </c>
       <c r="B12" s="43">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C12" s="16">
         <v>3.2199999999999999E-2</v>
@@ -4930,7 +4930,7 @@
         <v>8</v>
       </c>
       <c r="B13" s="43">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C13" s="16">
         <v>2.8000000000000001E-2</v>
@@ -5061,7 +5061,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="43">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C14" s="16">
         <v>2.98E-2</v>
@@ -5192,7 +5192,7 @@
         <v>10</v>
       </c>
       <c r="B15" s="43">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C15" s="16">
         <v>1.9900000000000001E-2</v>
@@ -5323,7 +5323,7 @@
         <v>11</v>
       </c>
       <c r="B16" s="43">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C16" s="16">
         <v>1.03E-2</v>
@@ -5454,7 +5454,7 @@
         <v>12</v>
       </c>
       <c r="B17" s="43">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C17" s="16">
         <v>2.1999999999999999E-2</v>
@@ -5585,7 +5585,7 @@
         <v>13</v>
       </c>
       <c r="B18" s="45">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C18" s="46">
         <v>1.5E-3</v>
@@ -5635,7 +5635,7 @@
         <v>14</v>
       </c>
       <c r="B19" s="14">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C19" s="16">
         <v>1.6999999999999999E-3</v>
@@ -5685,7 +5685,7 @@
         <v>15</v>
       </c>
       <c r="B20" s="14">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C20" s="16">
         <v>1.6999999999999999E-3</v>
@@ -5735,7 +5735,7 @@
         <v>16</v>
       </c>
       <c r="B21" s="51">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C21" s="18">
         <v>1.2500000000000001E-2</v>
@@ -6733,7 +6733,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -6754,7 +6754,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="1">
-        <v>30000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="3" spans="1:2">

</xml_diff>